<commit_message>
continue working through xml problems as a result of fixing xml comparison
</commit_message>
<xml_diff>
--- a/tests/data/9_default-excel.xlsx
+++ b/tests/data/9_default-excel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/xlsx/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
@@ -15,11 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -327,12 +317,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>